<commit_message>
Fix test identifier for 9.3.2.5
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV-I_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV-I_ICAM_Test_Cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D784D534-C04A-4E60-98D5-3A612C45A971}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3EF5A7-7234-4986-85D6-BB292FF3BECC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="1605" windowWidth="26190" windowHeight="12315" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3777" uniqueCount="1308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3777" uniqueCount="1309">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3959,6 +3959,9 @@
   </si>
   <si>
     <t>The Patron Header Version field has a value of 0x03.</t>
+  </si>
+  <si>
+    <t>9.3.2.5</t>
   </si>
 </sst>
 </file>
@@ -4802,13 +4805,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="13.75" style="4" customWidth="1"/>
-    <col min="2" max="2" width="57.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.69921875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="57.3984375" style="4" customWidth="1"/>
     <col min="3" max="5" width="10.5" style="4" customWidth="1"/>
-    <col min="6" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="17" customWidth="1"/>
+    <col min="6" max="256" width="8.8984375" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.8984375" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -5465,7 +5468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="31.5">
+    <row r="74" spans="1:5" ht="31.2">
       <c r="A74" s="3" t="s">
         <v>197</v>
       </c>
@@ -5553,7 +5556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="31.5">
+    <row r="85" spans="1:2" ht="31.2">
       <c r="A85" s="3" t="s">
         <v>208</v>
       </c>
@@ -5641,7 +5644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="31.5">
+    <row r="96" spans="1:2" ht="31.2">
       <c r="A96" s="3" t="s">
         <v>219</v>
       </c>
@@ -5729,7 +5732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" ht="31.2">
       <c r="A107" s="3" t="s">
         <v>230</v>
       </c>
@@ -5785,7 +5788,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="31.5">
+    <row r="114" spans="1:2" ht="31.2">
       <c r="A114" s="3" t="s">
         <v>244</v>
       </c>
@@ -5801,7 +5804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="28.5">
+    <row r="116" spans="1:2" ht="27.6">
       <c r="A116" s="3" t="s">
         <v>247</v>
       </c>
@@ -5841,7 +5844,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="47.25">
+    <row r="121" spans="1:2" ht="46.8">
       <c r="A121" s="3" t="s">
         <v>256</v>
       </c>
@@ -5857,7 +5860,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="63">
+    <row r="123" spans="1:2" ht="62.4">
       <c r="A123" s="3" t="s">
         <v>261</v>
       </c>
@@ -6009,7 +6012,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="31.5">
+    <row r="142" spans="1:2" ht="31.2">
       <c r="A142" s="3" t="s">
         <v>284</v>
       </c>
@@ -6025,7 +6028,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="31.5">
+    <row r="144" spans="1:2" ht="31.2">
       <c r="A144" s="3" t="s">
         <v>288</v>
       </c>
@@ -6033,7 +6036,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="47.25">
+    <row r="145" spans="1:2" ht="46.8">
       <c r="A145" s="3" t="s">
         <v>290</v>
       </c>
@@ -6041,7 +6044,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="47.25">
+    <row r="146" spans="1:2" ht="46.8">
       <c r="A146" s="3" t="s">
         <v>292</v>
       </c>
@@ -6065,7 +6068,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="47.25">
+    <row r="149" spans="1:2" ht="46.8">
       <c r="A149" s="3" t="s">
         <v>298</v>
       </c>
@@ -6081,7 +6084,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="63">
+    <row r="151" spans="1:2" ht="62.4">
       <c r="A151" s="3" t="s">
         <v>302</v>
       </c>
@@ -6089,7 +6092,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="31.5">
+    <row r="152" spans="1:2" ht="31.2">
       <c r="A152" s="3" t="s">
         <v>304</v>
       </c>
@@ -6097,7 +6100,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="31.5">
+    <row r="153" spans="1:2" ht="31.2">
       <c r="A153" s="3" t="s">
         <v>306</v>
       </c>
@@ -6161,7 +6164,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="31.5">
+    <row r="161" spans="1:2" ht="31.2">
       <c r="A161" s="3" t="s">
         <v>314</v>
       </c>
@@ -6177,7 +6180,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="31.5">
+    <row r="163" spans="1:2" ht="31.2">
       <c r="A163" s="3" t="s">
         <v>316</v>
       </c>
@@ -6185,7 +6188,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="31.5">
+    <row r="164" spans="1:2" ht="31.2">
       <c r="A164" s="3" t="s">
         <v>317</v>
       </c>
@@ -6193,7 +6196,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="47.25">
+    <row r="165" spans="1:2" ht="46.8">
       <c r="A165" s="3" t="s">
         <v>319</v>
       </c>
@@ -6217,7 +6220,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="31.5">
+    <row r="168" spans="1:2" ht="31.2">
       <c r="A168" s="3" t="s">
         <v>323</v>
       </c>
@@ -6233,7 +6236,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="63">
+    <row r="170" spans="1:2" ht="62.4">
       <c r="A170" s="3" t="s">
         <v>327</v>
       </c>
@@ -6241,7 +6244,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="31.5">
+    <row r="171" spans="1:2" ht="31.2">
       <c r="A171" s="3" t="s">
         <v>328</v>
       </c>
@@ -6249,7 +6252,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="31.5">
+    <row r="172" spans="1:2" ht="31.2">
       <c r="A172" s="3" t="s">
         <v>329</v>
       </c>
@@ -6345,7 +6348,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="47.25">
+    <row r="184" spans="1:2" ht="46.8">
       <c r="A184" s="3" t="s">
         <v>319</v>
       </c>
@@ -6361,7 +6364,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" ht="31.2">
       <c r="A186" s="3" t="s">
         <v>344</v>
       </c>
@@ -6369,7 +6372,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="31.5">
+    <row r="187" spans="1:2" ht="31.2">
       <c r="A187" s="3" t="s">
         <v>346</v>
       </c>
@@ -6385,7 +6388,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="63">
+    <row r="189" spans="1:2" ht="62.4">
       <c r="A189" s="3" t="s">
         <v>349</v>
       </c>
@@ -6393,7 +6396,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="31.5">
+    <row r="190" spans="1:2" ht="31.2">
       <c r="A190" s="3" t="s">
         <v>350</v>
       </c>
@@ -6401,7 +6404,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="31.5">
+    <row r="191" spans="1:2" ht="31.2">
       <c r="A191" s="3" t="s">
         <v>351</v>
       </c>
@@ -6449,7 +6452,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="47.25">
+    <row r="197" spans="1:2" ht="46.8">
       <c r="A197" s="3" t="s">
         <v>361</v>
       </c>
@@ -6457,7 +6460,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="47.25">
+    <row r="198" spans="1:2" ht="46.8">
       <c r="A198" s="3" t="s">
         <v>363</v>
       </c>
@@ -6481,7 +6484,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="31.5">
+    <row r="201" spans="1:2" ht="31.2">
       <c r="A201" s="3" t="s">
         <v>368</v>
       </c>
@@ -6489,7 +6492,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="31.5">
+    <row r="202" spans="1:2" ht="31.2">
       <c r="A202" s="3" t="s">
         <v>370</v>
       </c>
@@ -6593,7 +6596,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="31.5">
+    <row r="215" spans="1:2" ht="31.2">
       <c r="A215" s="3" t="s">
         <v>395</v>
       </c>
@@ -6737,7 +6740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="47.25">
+    <row r="233" spans="1:2" ht="46.8">
       <c r="A233" s="3" t="s">
         <v>417</v>
       </c>
@@ -6753,7 +6756,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="31.5">
+    <row r="235" spans="1:2" ht="31.2">
       <c r="A235" s="3" t="s">
         <v>423</v>
       </c>
@@ -6761,7 +6764,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="31.5">
+    <row r="236" spans="1:2" ht="31.2">
       <c r="A236" s="3" t="s">
         <v>426</v>
       </c>
@@ -6777,7 +6780,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" ht="31.2">
       <c r="A238" s="3" t="s">
         <v>432</v>
       </c>
@@ -6785,7 +6788,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="47.25">
+    <row r="239" spans="1:2" ht="62.4">
       <c r="A239" s="3" t="s">
         <v>435</v>
       </c>
@@ -6793,7 +6796,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="47.25">
+    <row r="240" spans="1:2" ht="46.8">
       <c r="A240" s="3" t="s">
         <v>438</v>
       </c>
@@ -6801,7 +6804,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="78.75">
+    <row r="241" spans="1:2" ht="78">
       <c r="A241" s="3" t="s">
         <v>441</v>
       </c>
@@ -6809,7 +6812,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="47.25">
+    <row r="242" spans="1:2" ht="62.4">
       <c r="A242" s="3" t="s">
         <v>444</v>
       </c>
@@ -6817,7 +6820,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="78.75">
+    <row r="243" spans="1:2" ht="78">
       <c r="A243" s="3" t="s">
         <v>447</v>
       </c>
@@ -6825,7 +6828,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="31.5">
+    <row r="244" spans="1:2" ht="31.2">
       <c r="A244" s="3" t="s">
         <v>450</v>
       </c>
@@ -6849,7 +6852,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="47.25">
+    <row r="247" spans="1:2" ht="46.8">
       <c r="A247" s="3" t="s">
         <v>455</v>
       </c>
@@ -6865,7 +6868,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="31.5">
+    <row r="249" spans="1:2" ht="31.2">
       <c r="A249" s="3" t="s">
         <v>459</v>
       </c>
@@ -6873,7 +6876,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="31.5">
+    <row r="250" spans="1:2" ht="31.2">
       <c r="A250" s="3" t="s">
         <v>461</v>
       </c>
@@ -6889,7 +6892,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" ht="31.2">
       <c r="A252" s="3" t="s">
         <v>464</v>
       </c>
@@ -6905,7 +6908,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="31.5">
+    <row r="254" spans="1:2" ht="31.2">
       <c r="A254" s="3" t="s">
         <v>467</v>
       </c>
@@ -6913,7 +6916,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="31.5">
+    <row r="255" spans="1:2" ht="31.2">
       <c r="A255" s="3" t="s">
         <v>469</v>
       </c>
@@ -6921,7 +6924,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="31.5">
+    <row r="256" spans="1:2" ht="31.2">
       <c r="A256" s="3" t="s">
         <v>472</v>
       </c>
@@ -6929,7 +6932,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="47.25">
+    <row r="257" spans="1:2" ht="46.8">
       <c r="A257" s="3" t="s">
         <v>474</v>
       </c>
@@ -6937,7 +6940,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="47.25">
+    <row r="258" spans="1:2" ht="62.4">
       <c r="A258" s="3" t="s">
         <v>477</v>
       </c>
@@ -6945,7 +6948,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="63">
+    <row r="259" spans="1:2" ht="62.4">
       <c r="A259" s="3" t="s">
         <v>479</v>
       </c>
@@ -6953,7 +6956,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="78.75">
+    <row r="260" spans="1:2" ht="78">
       <c r="A260" s="3" t="s">
         <v>481</v>
       </c>
@@ -6961,7 +6964,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="78.75">
+    <row r="261" spans="1:2" ht="78">
       <c r="A261" s="3" t="s">
         <v>483</v>
       </c>
@@ -6969,7 +6972,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="47.25">
+    <row r="262" spans="1:2" ht="46.8">
       <c r="A262" s="3" t="s">
         <v>486</v>
       </c>
@@ -6993,7 +6996,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="47.25">
+    <row r="265" spans="1:2" ht="46.8">
       <c r="A265" s="3" t="s">
         <v>490</v>
       </c>
@@ -7009,7 +7012,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="31.5">
+    <row r="267" spans="1:2" ht="31.2">
       <c r="A267" s="3" t="s">
         <v>492</v>
       </c>
@@ -7017,7 +7020,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="31.5">
+    <row r="268" spans="1:2" ht="31.2">
       <c r="A268" s="3" t="s">
         <v>493</v>
       </c>
@@ -7033,7 +7036,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" ht="31.2">
       <c r="A270" s="3" t="s">
         <v>495</v>
       </c>
@@ -7049,7 +7052,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="31.5">
+    <row r="272" spans="1:2" ht="31.2">
       <c r="A272" s="3" t="s">
         <v>497</v>
       </c>
@@ -7057,7 +7060,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="31.5">
+    <row r="273" spans="1:2" ht="31.2">
       <c r="A273" s="3" t="s">
         <v>498</v>
       </c>
@@ -7065,7 +7068,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="31.5">
+    <row r="274" spans="1:2" ht="31.2">
       <c r="A274" s="3" t="s">
         <v>499</v>
       </c>
@@ -7073,7 +7076,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="47.25">
+    <row r="275" spans="1:2" ht="46.8">
       <c r="A275" s="3" t="s">
         <v>500</v>
       </c>
@@ -7081,7 +7084,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="276" spans="1:2" ht="47.25">
+    <row r="276" spans="1:2" ht="62.4">
       <c r="A276" s="3" t="s">
         <v>501</v>
       </c>
@@ -7089,7 +7092,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="277" spans="1:2" ht="63">
+    <row r="277" spans="1:2" ht="62.4">
       <c r="A277" s="3" t="s">
         <v>502</v>
       </c>
@@ -7097,7 +7100,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="78.75">
+    <row r="278" spans="1:2" ht="78">
       <c r="A278" s="3" t="s">
         <v>503</v>
       </c>
@@ -7105,7 +7108,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="78.75">
+    <row r="279" spans="1:2" ht="78">
       <c r="A279" s="3" t="s">
         <v>504</v>
       </c>
@@ -7113,7 +7116,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="280" spans="1:2" ht="47.25">
+    <row r="280" spans="1:2" ht="46.8">
       <c r="A280" s="3" t="s">
         <v>505</v>
       </c>
@@ -7137,7 +7140,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="31.5">
+    <row r="283" spans="1:2" ht="31.2">
       <c r="A283" s="3" t="s">
         <v>507</v>
       </c>
@@ -7153,7 +7156,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="31.5">
+    <row r="285" spans="1:2" ht="31.2">
       <c r="A285" s="3" t="s">
         <v>511</v>
       </c>
@@ -7177,7 +7180,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="47.25">
+    <row r="288" spans="1:2" ht="46.8">
       <c r="A288" s="3" t="s">
         <v>519</v>
       </c>
@@ -7201,7 +7204,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="78.75">
+    <row r="291" spans="1:2" ht="78">
       <c r="A291" s="3" t="s">
         <v>527</v>
       </c>
@@ -7225,7 +7228,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="47.25">
+    <row r="294" spans="1:2" ht="46.8">
       <c r="A294" s="3" t="s">
         <v>531</v>
       </c>
@@ -7241,7 +7244,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="31.5">
+    <row r="296" spans="1:2" ht="31.2">
       <c r="A296" s="3" t="s">
         <v>533</v>
       </c>
@@ -7249,7 +7252,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="31.5">
+    <row r="297" spans="1:2" ht="31.2">
       <c r="A297" s="3" t="s">
         <v>534</v>
       </c>
@@ -7265,7 +7268,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" ht="31.2">
       <c r="A299" s="3" t="s">
         <v>536</v>
       </c>
@@ -7281,7 +7284,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="31.5">
+    <row r="301" spans="1:2" ht="31.2">
       <c r="A301" s="3" t="s">
         <v>538</v>
       </c>
@@ -7289,7 +7292,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="31.5">
+    <row r="302" spans="1:2" ht="31.2">
       <c r="A302" s="3" t="s">
         <v>539</v>
       </c>
@@ -7297,7 +7300,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="31.5">
+    <row r="303" spans="1:2" ht="31.2">
       <c r="A303" s="3" t="s">
         <v>540</v>
       </c>
@@ -7305,7 +7308,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="47.25">
+    <row r="304" spans="1:2" ht="46.8">
       <c r="A304" s="3" t="s">
         <v>541</v>
       </c>
@@ -7313,7 +7316,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="305" spans="1:2" ht="47.25">
+    <row r="305" spans="1:2" ht="62.4">
       <c r="A305" s="3" t="s">
         <v>542</v>
       </c>
@@ -7321,7 +7324,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="306" spans="1:2" ht="63">
+    <row r="306" spans="1:2" ht="62.4">
       <c r="A306" s="3" t="s">
         <v>543</v>
       </c>
@@ -7329,7 +7332,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="307" spans="1:2" ht="78.75">
+    <row r="307" spans="1:2" ht="78">
       <c r="A307" s="3" t="s">
         <v>544</v>
       </c>
@@ -7337,7 +7340,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="308" spans="1:2" ht="78.75">
+    <row r="308" spans="1:2" ht="78">
       <c r="A308" s="3" t="s">
         <v>545</v>
       </c>
@@ -7345,7 +7348,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="47.25">
+    <row r="309" spans="1:2" ht="46.8">
       <c r="A309" s="3" t="s">
         <v>546</v>
       </c>
@@ -7377,7 +7380,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="94.5">
+    <row r="313" spans="1:2" ht="93.6">
       <c r="A313" s="3" t="s">
         <v>548</v>
       </c>
@@ -7385,7 +7388,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="31.5">
+    <row r="314" spans="1:2" ht="31.2">
       <c r="A314" s="3" t="s">
         <v>550</v>
       </c>
@@ -7433,7 +7436,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="31.5">
+    <row r="320" spans="1:2" ht="31.2">
       <c r="A320" s="3" t="s">
         <v>564</v>
       </c>
@@ -7465,7 +7468,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="31.5">
+    <row r="324" spans="1:2" ht="46.8">
       <c r="A324" s="3" t="s">
         <v>575</v>
       </c>
@@ -7481,7 +7484,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="326" spans="1:2" ht="31.5">
+    <row r="326" spans="1:2" ht="31.2">
       <c r="A326" s="3" t="s">
         <v>581</v>
       </c>
@@ -7497,7 +7500,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="63">
+    <row r="328" spans="1:2" ht="62.4">
       <c r="A328" s="3" t="s">
         <v>587</v>
       </c>
@@ -7505,7 +7508,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="329" spans="1:2" ht="47.25">
+    <row r="329" spans="1:2" ht="46.8">
       <c r="A329" s="3" t="s">
         <v>589</v>
       </c>
@@ -7521,7 +7524,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="331" spans="1:2" ht="31.5">
+    <row r="331" spans="1:2" ht="31.2">
       <c r="A331" s="3" t="s">
         <v>593</v>
       </c>
@@ -7529,7 +7532,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="332" spans="1:2" ht="31.5">
+    <row r="332" spans="1:2" ht="31.2">
       <c r="A332" s="3" t="s">
         <v>596</v>
       </c>
@@ -7585,7 +7588,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="31.5">
+    <row r="339" spans="1:2" ht="31.2">
       <c r="A339" s="3" t="s">
         <v>610</v>
       </c>
@@ -7625,7 +7628,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="94.5">
+    <row r="344" spans="1:2" ht="93.6">
       <c r="A344" s="3" t="s">
         <v>618</v>
       </c>
@@ -7633,7 +7636,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="31.5">
+    <row r="345" spans="1:2" ht="31.2">
       <c r="A345" s="3" t="s">
         <v>619</v>
       </c>
@@ -7681,7 +7684,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="31.5">
+    <row r="351" spans="1:2" ht="31.2">
       <c r="A351" s="3" t="s">
         <v>631</v>
       </c>
@@ -7689,7 +7692,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="31.5">
+    <row r="352" spans="1:2" ht="31.2">
       <c r="A352" s="3" t="s">
         <v>633</v>
       </c>
@@ -7697,7 +7700,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="31.5">
+    <row r="353" spans="1:2" ht="31.2">
       <c r="A353" s="3" t="s">
         <v>635</v>
       </c>
@@ -7705,7 +7708,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="354" spans="1:2" ht="31.5">
+    <row r="354" spans="1:2" ht="46.8">
       <c r="A354" s="3" t="s">
         <v>637</v>
       </c>
@@ -7761,7 +7764,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="31.5">
+    <row r="361" spans="1:2" ht="31.2">
       <c r="A361" s="3" t="s">
         <v>646</v>
       </c>
@@ -7801,7 +7804,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="78.75">
+    <row r="366" spans="1:2" ht="78">
       <c r="A366" s="3" t="s">
         <v>650</v>
       </c>
@@ -7809,7 +7812,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="31.5">
+    <row r="367" spans="1:2" ht="31.2">
       <c r="A367" s="3" t="s">
         <v>652</v>
       </c>
@@ -7841,7 +7844,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="31.5">
+    <row r="371" spans="1:2" ht="31.2">
       <c r="A371" s="3" t="s">
         <v>658</v>
       </c>
@@ -7849,7 +7852,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="31.5">
+    <row r="372" spans="1:2" ht="31.2">
       <c r="A372" s="3" t="s">
         <v>660</v>
       </c>
@@ -7865,7 +7868,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="31.5">
+    <row r="374" spans="1:2" ht="31.2">
       <c r="A374" s="3" t="s">
         <v>665</v>
       </c>
@@ -7873,7 +7876,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="31.5">
+    <row r="375" spans="1:2" ht="31.2">
       <c r="A375" s="3" t="s">
         <v>667</v>
       </c>
@@ -7881,7 +7884,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="31.5">
+    <row r="376" spans="1:2" ht="46.8">
       <c r="A376" s="3" t="s">
         <v>669</v>
       </c>
@@ -7937,7 +7940,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="383" spans="1:2" ht="31.5">
+    <row r="383" spans="1:2" ht="31.2">
       <c r="A383" s="3" t="s">
         <v>676</v>
       </c>
@@ -7977,7 +7980,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="388" spans="1:2" ht="78.75">
+    <row r="388" spans="1:2" ht="78">
       <c r="A388" s="3" t="s">
         <v>680</v>
       </c>
@@ -7985,7 +7988,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="389" spans="1:2" ht="31.5">
+    <row r="389" spans="1:2" ht="31.2">
       <c r="A389" s="3" t="s">
         <v>681</v>
       </c>
@@ -8041,7 +8044,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="396" spans="1:2" ht="31.5">
+    <row r="396" spans="1:2" ht="31.2">
       <c r="A396" s="3" t="s">
         <v>691</v>
       </c>
@@ -8065,7 +8068,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="399" spans="1:2" ht="31.5">
+    <row r="399" spans="1:2" ht="31.2">
       <c r="A399" s="3" t="s">
         <v>698</v>
       </c>
@@ -8105,7 +8108,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="404" spans="1:2" ht="31.5">
+    <row r="404" spans="1:2" ht="31.2">
       <c r="A404" s="3" t="s">
         <v>707</v>
       </c>
@@ -8129,7 +8132,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="31.5">
+    <row r="407" spans="1:2" ht="31.2">
       <c r="A407" s="3" t="s">
         <v>710</v>
       </c>
@@ -8145,7 +8148,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="63">
+    <row r="409" spans="1:2" ht="62.4">
       <c r="A409" s="3" t="s">
         <v>712</v>
       </c>
@@ -8153,7 +8156,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="410" spans="1:2" ht="47.25">
+    <row r="410" spans="1:2" ht="46.8">
       <c r="A410" s="3" t="s">
         <v>713</v>
       </c>
@@ -8169,7 +8172,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="412" spans="1:2" ht="31.5">
+    <row r="412" spans="1:2" ht="31.2">
       <c r="A412" s="3" t="s">
         <v>716</v>
       </c>
@@ -8225,7 +8228,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="419" spans="1:2" ht="31.5">
+    <row r="419" spans="1:2" ht="31.2">
       <c r="A419" s="3" t="s">
         <v>723</v>
       </c>
@@ -8321,7 +8324,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="431" spans="1:2" ht="78.75">
+    <row r="431" spans="1:2" ht="78">
       <c r="A431" s="3" t="s">
         <v>732</v>
       </c>
@@ -8329,7 +8332,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="432" spans="1:2" ht="31.5">
+    <row r="432" spans="1:2" ht="31.2">
       <c r="A432" s="3" t="s">
         <v>733</v>
       </c>
@@ -8385,7 +8388,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="439" spans="1:2" ht="31.5">
+    <row r="439" spans="1:2" ht="31.2">
       <c r="A439" s="3" t="s">
         <v>742</v>
       </c>
@@ -8393,7 +8396,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="440" spans="1:2" ht="47.25">
+    <row r="440" spans="1:2" ht="46.8">
       <c r="A440" s="3" t="s">
         <v>744</v>
       </c>
@@ -8457,7 +8460,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="448" spans="1:2" ht="31.5">
+    <row r="448" spans="1:2" ht="31.2">
       <c r="A448" s="3" t="s">
         <v>753</v>
       </c>
@@ -8496,24 +8499,24 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B209" sqref="B209"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="14.25" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.19921875" style="4" customWidth="1"/>
     <col min="2" max="2" width="12" style="4" customWidth="1"/>
-    <col min="3" max="3" width="43.75" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.69921875" style="4" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.125" style="37" customWidth="1"/>
-    <col min="6" max="6" width="58.75" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.09765625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="58.69921875" style="4" customWidth="1"/>
     <col min="7" max="7" width="36.5" style="34" customWidth="1"/>
     <col min="8" max="1026" width="8.5" style="17" customWidth="1"/>
     <col min="1027" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="33" customFormat="1" ht="18.75">
+    <row r="1" spans="1:7" s="33" customFormat="1" ht="18">
       <c r="A1" s="38" t="s">
         <v>52</v>
       </c>
@@ -11727,7 +11730,7 @@
       <c r="F174" s="42"/>
       <c r="G174" s="42"/>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" ht="30">
       <c r="A175" s="42" t="s">
         <v>56</v>
       </c>
@@ -12048,7 +12051,7 @@
       <c r="F193" s="42"/>
       <c r="G193" s="42"/>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" ht="30">
       <c r="A194" s="42" t="s">
         <v>56</v>
       </c>
@@ -12306,7 +12309,7 @@
         <v>56</v>
       </c>
       <c r="B209" s="42" t="s">
-        <v>319</v>
+        <v>1308</v>
       </c>
       <c r="C209" s="42" t="s">
         <v>293</v>
@@ -12369,7 +12372,7 @@
       <c r="F212" s="42"/>
       <c r="G212" s="42"/>
     </row>
-    <row r="213" spans="1:7">
+    <row r="213" spans="1:7" ht="30">
       <c r="A213" s="42" t="s">
         <v>56</v>
       </c>
@@ -13215,7 +13218,7 @@
       <c r="F262" s="42"/>
       <c r="G262" s="47"/>
     </row>
-    <row r="263" spans="1:7" ht="60">
+    <row r="263" spans="1:7" ht="75">
       <c r="A263" s="42" t="s">
         <v>56</v>
       </c>
@@ -14027,7 +14030,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="311" spans="1:7">
+    <row r="311" spans="1:7" ht="30">
       <c r="A311" s="42" t="s">
         <v>56</v>
       </c>
@@ -14061,7 +14064,7 @@
       <c r="F312" s="42"/>
       <c r="G312" s="47"/>
     </row>
-    <row r="313" spans="1:7" ht="45">
+    <row r="313" spans="1:7" ht="60">
       <c r="A313" s="42" t="s">
         <v>56</v>
       </c>
@@ -17026,14 +17029,14 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="45.125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="4" customWidth="1"/>
-    <col min="4" max="5" width="81.375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="45.09765625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" style="4" customWidth="1"/>
+    <col min="4" max="5" width="81.3984375" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.8984375" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -17119,7 +17122,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="126">
+    <row r="5" spans="1:7" ht="140.4">
       <c r="A5" s="3" t="s">
         <v>68</v>
       </c>
@@ -17173,15 +17176,15 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="68.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.8984375" style="4" customWidth="1"/>
     <col min="4" max="4" width="100" style="4" customWidth="1"/>
-    <col min="5" max="6" width="22.875" style="4" customWidth="1"/>
+    <col min="5" max="6" width="22.8984375" style="4" customWidth="1"/>
     <col min="7" max="7" width="20" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.8984375" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -17322,7 +17325,7 @@
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="31.5">
+    <row r="8" spans="1:7" ht="31.2">
       <c r="A8" s="6" t="s">
         <v>784</v>
       </c>
@@ -17875,7 +17878,7 @@
       </c>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" ht="63">
+    <row r="37" spans="1:7" ht="78">
       <c r="A37" s="6" t="s">
         <v>246</v>
       </c>
@@ -17896,7 +17899,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="31.5">
+    <row r="38" spans="1:7" ht="31.2">
       <c r="A38" s="6" t="s">
         <v>509</v>
       </c>
@@ -17972,7 +17975,7 @@
       </c>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:7" ht="47.25">
+    <row r="42" spans="1:7" ht="46.8">
       <c r="A42" s="6" t="s">
         <v>263</v>
       </c>
@@ -18256,19 +18259,19 @@
       <selection sqref="A1:D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="29" customWidth="1"/>
-    <col min="2" max="2" width="47.375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="4" customWidth="1"/>
-    <col min="4" max="5" width="80.875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.8984375" style="29" customWidth="1"/>
+    <col min="2" max="2" width="47.3984375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.8984375" style="4" customWidth="1"/>
+    <col min="4" max="5" width="80.8984375" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="17" customWidth="1"/>
+    <col min="8" max="256" width="8.8984375" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.8984375" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="24" customFormat="1" ht="30.95" customHeight="1">
+    <row r="1" spans="1:256" s="24" customFormat="1" ht="30.9" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>756</v>
       </c>
@@ -19262,7 +19265,7 @@
       </c>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" ht="30.95" customHeight="1">
+    <row r="40" spans="1:7" ht="30.9" customHeight="1">
       <c r="A40" s="6" t="s">
         <v>924</v>
       </c>
@@ -19315,7 +19318,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:7" ht="30.95" customHeight="1">
+    <row r="43" spans="1:7" ht="30.9" customHeight="1">
       <c r="A43" s="6" t="s">
         <v>934</v>
       </c>
@@ -19423,7 +19426,7 @@
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:256" s="32" customFormat="1" ht="31.5">
+    <row r="49" spans="1:256" s="32" customFormat="1" ht="31.2">
       <c r="A49" s="57" t="s">
         <v>955</v>
       </c>
@@ -19721,17 +19724,17 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="33.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="44.375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="41.375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="44.3984375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" style="4" customWidth="1"/>
     <col min="7" max="7" width="29" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="17" customWidth="1"/>
+    <col min="8" max="256" width="8.8984375" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.8984375" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -20201,7 +20204,7 @@
       <c r="F24" s="58"/>
       <c r="G24" s="58"/>
     </row>
-    <row r="25" spans="1:7" ht="45">
+    <row r="25" spans="1:7" ht="43.2">
       <c r="A25" s="58" t="s">
         <v>1213</v>
       </c>
@@ -20218,7 +20221,7 @@
       <c r="F25" s="58"/>
       <c r="G25" s="58"/>
     </row>
-    <row r="26" spans="1:7" ht="30">
+    <row r="26" spans="1:7" ht="28.8">
       <c r="A26" s="58" t="s">
         <v>1267</v>
       </c>
@@ -20235,7 +20238,7 @@
       <c r="F26" s="58"/>
       <c r="G26" s="58"/>
     </row>
-    <row r="27" spans="1:7" ht="30">
+    <row r="27" spans="1:7" ht="28.8">
       <c r="A27" s="58" t="s">
         <v>1270</v>
       </c>
@@ -20252,7 +20255,7 @@
       <c r="F27" s="58"/>
       <c r="G27" s="58"/>
     </row>
-    <row r="28" spans="1:7" ht="30">
+    <row r="28" spans="1:7" ht="28.8">
       <c r="A28" s="58" t="s">
         <v>1273</v>
       </c>
@@ -20269,7 +20272,7 @@
       <c r="F28" s="58"/>
       <c r="G28" s="58"/>
     </row>
-    <row r="29" spans="1:7" ht="30">
+    <row r="29" spans="1:7" ht="28.8">
       <c r="A29" s="58" t="s">
         <v>1276</v>
       </c>
@@ -20286,7 +20289,7 @@
       <c r="F29" s="58"/>
       <c r="G29" s="58"/>
     </row>
-    <row r="30" spans="1:7" ht="30">
+    <row r="30" spans="1:7" ht="28.8">
       <c r="A30" s="58" t="s">
         <v>1279</v>
       </c>
@@ -20321,18 +20324,18 @@
       <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9" style="17"/>
-    <col min="2" max="2" width="54.125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="17.75" style="4" customWidth="1"/>
-    <col min="4" max="4" width="54.625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="103.875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="35.625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="75.625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="54.09765625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="17.69921875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="54.59765625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="103.8984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="35.59765625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="75.59765625" style="4" customWidth="1"/>
     <col min="8" max="9" width="10.5" style="4" customWidth="1"/>
-    <col min="10" max="258" width="8.875" style="4" customWidth="1"/>
-    <col min="259" max="1027" width="8.875" style="17" customWidth="1"/>
+    <col min="10" max="258" width="8.8984375" style="4" customWidth="1"/>
+    <col min="259" max="1027" width="8.8984375" style="17" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -20411,7 +20414,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="78.75">
+    <row r="4" spans="1:9" ht="78">
       <c r="A4" s="55" t="s">
         <v>1002</v>
       </c>
@@ -20450,17 +20453,17 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="53.375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="53.3984375" style="18" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="18" customWidth="1"/>
     <col min="4" max="4" width="44.5" style="18" customWidth="1"/>
-    <col min="5" max="5" width="31.875" style="18" customWidth="1"/>
-    <col min="6" max="6" width="11.875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="31.8984375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="11.8984375" style="18" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="18" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="18" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="8" max="256" width="8.8984375" style="18" customWidth="1"/>
+    <col min="257" max="1025" width="8.8984375" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
@@ -21159,7 +21162,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="23" spans="1:256" s="36" customFormat="1" ht="31.5">
+    <row r="23" spans="1:256" s="36" customFormat="1" ht="31.2">
       <c r="A23" s="6" t="s">
         <v>1069</v>
       </c>
@@ -21957,7 +21960,7 @@
       <c r="IU25" s="35"/>
       <c r="IV25" s="35"/>
     </row>
-    <row r="26" spans="1:256" s="36" customFormat="1" ht="31.5">
+    <row r="26" spans="1:256" s="36" customFormat="1" ht="31.2">
       <c r="A26" s="6" t="s">
         <v>1065</v>
       </c>
@@ -22507,15 +22510,15 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.5" style="22" customWidth="1"/>
-    <col min="2" max="2" width="53.375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="53.3984375" style="17" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="17" customWidth="1"/>
     <col min="4" max="5" width="44.5" style="17" customWidth="1"/>
-    <col min="6" max="6" width="11.875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="11.8984375" style="17" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="17" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="17" customWidth="1"/>
+    <col min="8" max="1025" width="8.8984375" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -22791,7 +22794,7 @@
       <c r="IU1" s="23"/>
       <c r="IV1" s="23"/>
     </row>
-    <row r="2" spans="1:256" ht="31.5">
+    <row r="2" spans="1:256" ht="31.2">
       <c r="A2" s="56" t="s">
         <v>1201</v>
       </c>
@@ -22812,7 +22815,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="31.5">
+    <row r="3" spans="1:256" ht="31.2">
       <c r="A3" s="56" t="s">
         <v>1292</v>
       </c>
@@ -22833,7 +22836,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:256" ht="31.5">
+    <row r="4" spans="1:256" ht="31.2">
       <c r="A4" s="6" t="s">
         <v>1295</v>
       </c>

</xml_diff>